<commit_message>
Added test cases to view active order
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint 1.xlsx
+++ b/Test-cases/Sprint 1.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="219"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="502" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="User Menu" sheetId="2" r:id="rId2"/>
+    <sheet name="Place Order" sheetId="3" r:id="rId3"/>
+    <sheet name="View Active order" sheetId="4" r:id="rId4"/>
+    <sheet name="Monitor Order" sheetId="5" r:id="rId5"/>
+    <sheet name="View History" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
   <si>
     <t>Username</t>
   </si>
@@ -141,6 +145,57 @@
   </si>
   <si>
     <t>Successfully logged in</t>
+  </si>
+  <si>
+    <t>Verify Employees can view current active order.</t>
+  </si>
+  <si>
+    <t>Employees are logged in to the application.</t>
+  </si>
+  <si>
+    <t>2. Application should display the list of active order.</t>
+  </si>
+  <si>
+    <t>4. Click ok.</t>
+  </si>
+  <si>
+    <t>Isconfirmed</t>
+  </si>
+  <si>
+    <t>IsDelivered</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>1. Click on Order</t>
+  </si>
+  <si>
+    <t>3. Select Isconfirmed/IsDelivered according to the various criteria below.</t>
+  </si>
+  <si>
+    <t>Test004</t>
+  </si>
+  <si>
+    <t>Test004.A</t>
+  </si>
+  <si>
+    <t>Test004.B</t>
+  </si>
+  <si>
+    <t>Test004.C</t>
+  </si>
+  <si>
+    <t>Test004.D</t>
+  </si>
+  <si>
+    <t>"Confirmation is sent to the customer" message is displayed. It still gets displayed in the order list.</t>
+  </si>
+  <si>
+    <t>"The order has been delivered" message is displayed. The order no longer appears in the order list.</t>
+  </si>
+  <si>
+    <t>"Confirmation is sent to the customer and the order has been delivered" message is displayed.  The order no longer appears in the order list.</t>
   </si>
 </sst>
 </file>
@@ -238,7 +293,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -288,13 +343,243 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="42">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -859,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -892,11 +1177,11 @@
       <c r="B3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
@@ -905,11 +1190,11 @@
       <c r="B4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
@@ -922,26 +1207,26 @@
       <c r="B6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="18"/>
     </row>
     <row r="8" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
@@ -952,38 +1237,38 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="17" t="s">
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -1177,83 +1462,74 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="11">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <conditionalFormatting sqref="F13:F21">
-    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F21">
+      <formula1>#REF!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>F13:F21</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1279,7 +1555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -1291,4 +1569,323 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="18"/>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="16">
+        <v>4</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E14:E17">
+    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Partially Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Partially Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14:E17">
+      <formula1>#REF!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test case for " Customer can monitor order"
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint 1.xlsx
+++ b/Test-cases/Sprint 1.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="502" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="502" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="User Menu" sheetId="2" r:id="rId2"/>
     <sheet name="Place Order" sheetId="3" r:id="rId3"/>
     <sheet name="View Active order" sheetId="4" r:id="rId4"/>
-    <sheet name="Monitor Order" sheetId="5" r:id="rId5"/>
+    <sheet name="Customer Monitor Order" sheetId="5" r:id="rId5"/>
     <sheet name="View History" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet4" sheetId="7" r:id="rId7"/>
   </sheets>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t>Username</t>
   </si>
@@ -196,6 +196,27 @@
   </si>
   <si>
     <t>"Confirmation is sent to the customer and the order has been delivered" message is displayed.  The order no longer appears in the order list.</t>
+  </si>
+  <si>
+    <t>Test005</t>
+  </si>
+  <si>
+    <t>Verify customer can monitor order.</t>
+  </si>
+  <si>
+    <t>Customer are logged in to the application.</t>
+  </si>
+  <si>
+    <t>1. Click on Myorder(Now Customer/Active)</t>
+  </si>
+  <si>
+    <t>Expected.</t>
+  </si>
+  <si>
+    <t>User is able to see list of order along with the status of the order.</t>
+  </si>
+  <si>
+    <t>Test Result :</t>
   </si>
 </sst>
 </file>
@@ -355,7 +376,455 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="98">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1475,46 +1944,46 @@
     <mergeCell ref="E11:E12"/>
   </mergeCells>
   <conditionalFormatting sqref="F13:F21">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1575,8 +2044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1795,46 +2264,46 @@
     <mergeCell ref="D12:D13"/>
   </mergeCells>
   <conditionalFormatting sqref="E14:E17">
-    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1850,15 +2319,179 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C9:D9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Partially Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Partially Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+      <formula1>#REF!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added test case for " User can see order history"
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint 1.xlsx
+++ b/Test-cases/Sprint 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="502" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="502" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="70">
   <si>
     <t>Username</t>
   </si>
@@ -217,6 +217,21 @@
   </si>
   <si>
     <t>Test Result :</t>
+  </si>
+  <si>
+    <t>Test006</t>
+  </si>
+  <si>
+    <t>Verify customer can view history.</t>
+  </si>
+  <si>
+    <t>1. Click on History(Now Customer/History)</t>
+  </si>
+  <si>
+    <t>2. Application should display the list of order.</t>
+  </si>
+  <si>
+    <t>User is able to see list order that has been delivered to them along with the order detail. The detail includes order name,date delivered and date ordered.</t>
   </si>
 </sst>
 </file>
@@ -376,7 +391,231 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="126">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1944,46 +2183,46 @@
     <mergeCell ref="E11:E12"/>
   </mergeCells>
   <conditionalFormatting sqref="F13:F21">
-    <cfRule type="cellIs" dxfId="69" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2264,46 +2503,46 @@
     <mergeCell ref="D12:D13"/>
   </mergeCells>
   <conditionalFormatting sqref="E14:E17">
-    <cfRule type="cellIs" dxfId="55" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2321,8 +2560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2408,6 +2647,184 @@
       </c>
       <c r="C9" s="18" t="s">
         <v>63</v>
+      </c>
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C9:D9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="55" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Partially Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Partially Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+      <formula1>#REF!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>69</v>
       </c>
       <c r="D9" s="18"/>
     </row>
@@ -2491,21 +2908,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Test for view current order
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint 1.xlsx
+++ b/Test-cases/Sprint 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="12180" tabRatio="502"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="12180" tabRatio="502" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
   <si>
     <t>Username</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>NOT OK</t>
+  </si>
+  <si>
+    <t>Test Results</t>
   </si>
 </sst>
 </file>
@@ -359,7 +362,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -397,9 +400,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -418,6 +418,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -426,119 +432,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="22"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="44"/>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="22"/>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="44"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="22"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="44"/>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="22"/>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="44"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1215,7 +1109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -1232,114 +1126,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="19" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>4</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="19" t="s">
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="18"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -1351,7 +1245,7 @@
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1374,7 +1268,7 @@
       <c r="C14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -1395,7 +1289,7 @@
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1418,7 +1312,7 @@
       <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="12" t="s">
@@ -1441,7 +1335,7 @@
       <c r="C17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="12" t="s">
@@ -1464,7 +1358,7 @@
       <c r="C18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="12" t="s">
@@ -1547,10 +1441,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F22" s="17"/>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F23" s="17"/>
+      <c r="F23" s="16"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -1633,138 +1527,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="14"/>
+    <col min="1" max="1" width="10.28515625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.140625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="19" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="19" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>4</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="18" t="s">
+      <c r="E12" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="18"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1776,15 +1666,15 @@
       <c r="D14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>8</v>
+      <c r="E14" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1796,15 +1686,15 @@
       <c r="D15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>8</v>
+      <c r="E15" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>53</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1816,15 +1706,15 @@
       <c r="D16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>8</v>
+      <c r="E16" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1834,10 +1724,12 @@
         <v>7</v>
       </c>
       <c r="D17" s="12"/>
-      <c r="E17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="10"/>
+      <c r="E17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1847,8 +1739,8 @@
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
@@ -1858,56 +1750,6 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="F12:F13"/>
   </mergeCells>
-  <conditionalFormatting sqref="E14:E17">
-    <cfRule type="cellIs" dxfId="41" priority="1" stopIfTrue="1" operator="equal">
-      <formula>"Not Tested"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Ongoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"Blocked"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Partially Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"Not Tested"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Ongoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Blocked"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Partially Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14:E17">
-      <formula1>#REF!</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1927,102 +1769,102 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="14"/>
+    <col min="1" max="1" width="10.28515625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
     </row>
     <row r="3" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2112,102 +1954,102 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="14"/>
+    <col min="1" max="1" width="10.28515625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
     </row>
     <row r="3" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tested customer monitor order
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint 1.xlsx
+++ b/Test-cases/Sprint 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="12180" tabRatio="502" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="12180" tabRatio="502" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -432,119 +432,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="22"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="44"/>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="22"/>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="44"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="22"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="44"/>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="22"/>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="44"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1527,7 +1415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -1763,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1861,11 +1749,11 @@
       <c r="B11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>8</v>
+      <c r="C11" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1885,56 +1773,6 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C9:D9"/>
   </mergeCells>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
-      <formula>"Not Tested"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Ongoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"Blocked"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Partially Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"Not Tested"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Ongoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Blocked"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Partially Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
-      <formula1>#REF!</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Test Updated For Sprint 1,2,3
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint 1.xlsx
+++ b/Test-cases/Sprint 1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="12180" tabRatio="502" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="640" yWindow="720" windowWidth="19440" windowHeight="12180" tabRatio="502" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,9 @@
     <sheet name="Place Order" sheetId="3" r:id="rId3"/>
     <sheet name="View Active order" sheetId="4" r:id="rId4"/>
     <sheet name="Customer Monitor Order" sheetId="5" r:id="rId5"/>
-    <sheet name="View History" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet4" sheetId="7" r:id="rId7"/>
+    <sheet name="Order Detail" sheetId="8" r:id="rId6"/>
+    <sheet name="View History" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
   <si>
     <t>Username</t>
   </si>
@@ -246,6 +247,30 @@
   </si>
   <si>
     <t>Test Results</t>
+  </si>
+  <si>
+    <t>Test204</t>
+  </si>
+  <si>
+    <t>Verify employee can view order detail</t>
+  </si>
+  <si>
+    <t>Order has been placed.</t>
+  </si>
+  <si>
+    <t>Employee has logged in.</t>
+  </si>
+  <si>
+    <t>Steps 1:</t>
+  </si>
+  <si>
+    <t>1. click on order</t>
+  </si>
+  <si>
+    <t>2. Click on view</t>
+  </si>
+  <si>
+    <t>1. Order detail with ordered time, delivery time, date created should be displayed</t>
   </si>
 </sst>
 </file>
@@ -314,7 +339,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +350,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="31"/>
         <bgColor indexed="44"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -359,7 +390,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -412,10 +443,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -813,7 +850,7 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
@@ -855,7 +892,7 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
@@ -882,87 +919,87 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="51" customHeight="1">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="25.5" customHeight="1">
       <c r="A6" s="14">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:7" ht="38.25" customHeight="1">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:7" ht="25.5" customHeight="1">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="19"/>
-    </row>
-    <row r="9" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:7" ht="25.5" customHeight="1">
       <c r="A9" s="14">
         <v>4</v>
       </c>
@@ -970,41 +1007,41 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="19" t="s">
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+    <row r="12" spans="1:7">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G12" s="19"/>
+    </row>
+    <row r="13" spans="1:7" ht="30.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -1027,7 +1064,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="27" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1048,7 +1085,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="27.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1071,7 +1108,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="28.5" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1094,7 +1131,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="30" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1117,7 +1154,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="29.25" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -1140,7 +1177,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="29.25" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1163,7 +1200,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="29.25" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -1186,7 +1223,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="28.5" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1209,29 +1246,28 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="F23" s="15"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="11">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1252,7 +1288,7 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1276,7 +1312,7 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1300,93 +1336,93 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.140625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="12"/>
+    <col min="1" max="1" width="10.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="50.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.1640625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="14" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="51" customHeight="1">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="25.5" customHeight="1">
       <c r="A6" s="14">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" ht="38.25" customHeight="1">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" customHeight="1">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="19"/>
-    </row>
-    <row r="9" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" customHeight="1">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" customHeight="1">
       <c r="A10" s="14">
         <v>4</v>
       </c>
@@ -1394,35 +1430,35 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="19" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
+    <row r="13" spans="1:6">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:6" ht="30.75" customHeight="1">
       <c r="A14" s="12" t="s">
         <v>50</v>
       </c>
@@ -1442,7 +1478,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="27" customHeight="1">
       <c r="A15" s="12" t="s">
         <v>51</v>
       </c>
@@ -1462,7 +1498,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="36">
       <c r="A16" s="12" t="s">
         <v>52</v>
       </c>
@@ -1482,7 +1518,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="28.5" customHeight="1">
       <c r="A17" s="12" t="s">
         <v>53</v>
       </c>
@@ -1500,24 +1536,24 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:6" ht="30" customHeight="1"/>
+    <row r="19" spans="1:6" ht="29.25" customHeight="1"/>
+    <row r="20" spans="1:6" ht="29.25" customHeight="1"/>
+    <row r="21" spans="1:6" ht="29.25" customHeight="1"/>
+    <row r="22" spans="1:6" ht="28.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1536,97 +1572,97 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="12"/>
+    <col min="1" max="1" width="10.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="50.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5" style="12" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="51" customHeight="1">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="25.5" customHeight="1">
       <c r="A6" s="14">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:5" ht="38.25" customHeight="1">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" customHeight="1">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
     </row>
-    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="25.5" customHeight="1">
       <c r="A9" s="14"/>
       <c r="B9" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" ht="25.5" customHeight="1">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="B11" s="14" t="s">
         <v>63</v>
       </c>
@@ -1637,15 +1673,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="14" spans="1:5" ht="30.75" customHeight="1"/>
+    <row r="15" spans="1:5" ht="27" customHeight="1"/>
+    <row r="17" ht="28.5" customHeight="1"/>
+    <row r="18" ht="30" customHeight="1"/>
+    <row r="19" ht="29.25" customHeight="1"/>
+    <row r="20" ht="29.25" customHeight="1"/>
+    <row r="21" ht="29.25" customHeight="1"/>
+    <row r="22" ht="28.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C3:E3"/>
@@ -1665,103 +1701,247 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="18" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="50.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="51.5" style="18" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="14"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="14">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="14">
+        <v>4</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="18">
+        <v>5</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="12"/>
+    <col min="1" max="1" width="10.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="50.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5" style="12" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="14" t="s">
         <v>64</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="51" customHeight="1">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="25.5" customHeight="1">
       <c r="A6" s="14">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:5" ht="38.25" customHeight="1">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" customHeight="1">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
     </row>
-    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="25.5" customHeight="1">
       <c r="A9" s="14"/>
       <c r="B9" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" ht="25.5" customHeight="1">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="B11" s="14" t="s">
         <v>63</v>
       </c>
@@ -1772,15 +1952,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="14" spans="1:5" ht="30.75" customHeight="1"/>
+    <row r="15" spans="1:5" ht="27" customHeight="1"/>
+    <row r="17" ht="28.5" customHeight="1"/>
+    <row r="18" ht="30" customHeight="1"/>
+    <row r="19" ht="29.25" customHeight="1"/>
+    <row r="20" ht="29.25" customHeight="1"/>
+    <row r="21" ht="29.25" customHeight="1"/>
+    <row r="22" ht="28.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C3:E3"/>
@@ -1798,7 +1978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1806,7 +1986,7 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Tested spring 1 in Mozilla
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint 1.xlsx
+++ b/Test-cases/Sprint 1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="720" windowWidth="19440" windowHeight="12180" tabRatio="502" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="645" yWindow="720" windowWidth="19440" windowHeight="12180" tabRatio="502" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="84">
   <si>
     <t>Username</t>
   </si>
@@ -41,12 +41,6 @@
   </si>
   <si>
     <t>Test Result</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>MM/DD/YYYY</t>
   </si>
   <si>
     <t>Blank</t>
@@ -271,6 +265,21 @@
   </si>
   <si>
     <t>1. Order detail with ordered time, delivery time, date created should be displayed</t>
+  </si>
+  <si>
+    <t>Remarks(chrome)</t>
+  </si>
+  <si>
+    <t>Remarks(Mozilla)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK </t>
+  </si>
+  <si>
+    <t>1. Tested(Chrome)</t>
+  </si>
+  <si>
+    <t>2. Tested(Mozilla)</t>
   </si>
 </sst>
 </file>
@@ -390,7 +399,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -446,13 +455,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -850,7 +862,7 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
@@ -892,7 +904,7 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
@@ -913,359 +925,390 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="19" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="51" customHeight="1">
+    <row r="3" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:7">
+        <v>12</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:7">
+        <v>14</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="25.5" customHeight="1">
+    <row r="6" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="20"/>
-    </row>
-    <row r="7" spans="1:7" ht="38.25" customHeight="1">
+        <v>17</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:7" ht="25.5" customHeight="1">
+      <c r="C7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="20"/>
-    </row>
-    <row r="9" spans="1:7" ht="25.5" customHeight="1">
+      <c r="C8" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
         <v>4</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="21" t="s">
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="3" t="s">
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="19"/>
-    </row>
-    <row r="13" spans="1:7" ht="30.75" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="27" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="D14" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="27.75" customHeight="1">
+        <v>68</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="7" t="s">
+      <c r="D18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="E19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A19" s="1" t="s">
+      <c r="E20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="B21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="E21" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>68</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F23" s="15"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="11">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
+  <mergeCells count="12">
+    <mergeCell ref="H11:H12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter alignWithMargins="0">
@@ -1288,7 +1331,7 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1309,10 +1352,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1330,230 +1373,247 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.1640625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="12"/>
+    <col min="1" max="1" width="10.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.140625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="19" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:6" ht="51" customHeight="1">
+    <row r="3" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="20"/>
-    </row>
-    <row r="5" spans="1:6">
+        <v>14</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:6" ht="25.5" customHeight="1">
+    <row r="6" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="20"/>
-    </row>
-    <row r="7" spans="1:6" ht="38.25" customHeight="1">
+        <v>17</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:6" ht="25.5" customHeight="1">
+      <c r="C7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="20"/>
-    </row>
-    <row r="9" spans="1:6" ht="25.5" customHeight="1">
+      <c r="C8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" spans="1:6" ht="25.5" customHeight="1">
+      <c r="C9" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
         <v>4</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A12" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="19" t="s">
+      <c r="C14" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="19"/>
-    </row>
-    <row r="14" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A14" s="12" t="s">
+      <c r="D14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="B16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="27" customHeight="1">
-      <c r="A15" s="12" t="s">
+      <c r="G16" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="36">
-      <c r="A16" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.5" customHeight="1">
-      <c r="A17" s="12" t="s">
-        <v>53</v>
-      </c>
       <c r="B17" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1"/>
-    <row r="19" spans="1:6" ht="29.25" customHeight="1"/>
-    <row r="20" spans="1:6" ht="29.25" customHeight="1"/>
-    <row r="21" spans="1:6" ht="29.25" customHeight="1"/>
-    <row r="22" spans="1:6" ht="28.5" customHeight="1"/>
+      <c r="G17" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
+  <mergeCells count="12">
+    <mergeCell ref="G12:G13"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1569,119 +1629,126 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5" style="12" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="12"/>
+    <col min="1" max="1" width="10.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:5" ht="51" customHeight="1">
+    <row r="3" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:5">
+        <v>14</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:5" ht="25.5" customHeight="1">
+    <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" ht="38.25" customHeight="1">
+        <v>17</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:5" ht="25.5" customHeight="1">
+      <c r="C7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
     </row>
-    <row r="9" spans="1:5" ht="25.5" customHeight="1">
+    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" spans="1:5" ht="25.5" customHeight="1">
+        <v>59</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="14" spans="1:5" ht="30.75" customHeight="1"/>
-    <row r="15" spans="1:5" ht="27" customHeight="1"/>
-    <row r="17" ht="28.5" customHeight="1"/>
-    <row r="18" ht="30" customHeight="1"/>
-    <row r="19" ht="29.25" customHeight="1"/>
-    <row r="20" ht="29.25" customHeight="1"/>
-    <row r="21" ht="29.25" customHeight="1"/>
-    <row r="22" ht="28.5" customHeight="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C3:E3"/>
@@ -1701,127 +1768,135 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="51.5" style="18" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="18"/>
+    <col min="1" max="1" width="10.28515625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="18" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-    </row>
-    <row r="4" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-    </row>
-    <row r="5" spans="1:6">
+        <v>14</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="20"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
         <v>3</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:6">
+        <v>75</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="20"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="C8" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
         <v>4</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="20"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="C10" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>5</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>71</v>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1847,120 +1922,127 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5" style="12" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="12"/>
+    <col min="1" max="1" width="10.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:5" ht="51" customHeight="1">
+    <row r="3" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:5">
+        <v>14</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:5" ht="25.5" customHeight="1">
+    <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" ht="38.25" customHeight="1">
+        <v>17</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:5" ht="25.5" customHeight="1">
+      <c r="C7" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
     </row>
-    <row r="9" spans="1:5" ht="25.5" customHeight="1">
+    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" spans="1:5" ht="25.5" customHeight="1">
+        <v>59</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="14" spans="1:5" ht="30.75" customHeight="1"/>
-    <row r="15" spans="1:5" ht="27" customHeight="1"/>
-    <row r="17" ht="28.5" customHeight="1"/>
-    <row r="18" ht="30" customHeight="1"/>
-    <row r="19" ht="29.25" customHeight="1"/>
-    <row r="20" ht="29.25" customHeight="1"/>
-    <row r="21" ht="29.25" customHeight="1"/>
-    <row r="22" ht="28.5" customHeight="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C3:E3"/>
@@ -1986,7 +2068,7 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
added missing tests for sprint 1
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint 1.xlsx
+++ b/Test-cases/Sprint 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="720" windowWidth="19440" windowHeight="12180" tabRatio="502" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="645" yWindow="720" windowWidth="19440" windowHeight="12180" tabRatio="502" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,16 +17,11 @@
     <sheet name="Sheet4" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="96">
   <si>
     <t>Username</t>
   </si>
@@ -280,6 +275,42 @@
   </si>
   <si>
     <t>2. Tested(Mozilla)</t>
+  </si>
+  <si>
+    <t>Test002</t>
+  </si>
+  <si>
+    <t>Test that a customer can view the menu</t>
+  </si>
+  <si>
+    <t>customer is logged in</t>
+  </si>
+  <si>
+    <t>1. Click on Menu/customer</t>
+  </si>
+  <si>
+    <t>1.Menu page should be displayed</t>
+  </si>
+  <si>
+    <t>Test003</t>
+  </si>
+  <si>
+    <t>Test that a customer can place an order</t>
+  </si>
+  <si>
+    <t>1.customer is logged in</t>
+  </si>
+  <si>
+    <t>2.Customer has clicked menu/customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add item to the cart. </t>
+  </si>
+  <si>
+    <t>2.Click on checkout.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Confirmation message should be displayed </t>
   </si>
 </sst>
 </file>
@@ -399,7 +430,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -465,6 +496,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1297,6 +1346,11 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="C3:E3"/>
@@ -1304,11 +1358,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter alignWithMargins="0">
@@ -1325,49 +1374,277 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="24"/>
+    </row>
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="26">
+        <v>3</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="26">
+        <v>4</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="25">
+        <v>5</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="5">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="30">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="28"/>
+    </row>
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="30">
+        <v>2</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="28"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="30">
+        <v>3</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="30">
+        <v>4</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+    </row>
+    <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="29">
+        <v>5</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="5">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1602,6 +1879,11 @@
     <row r="22" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C3:D3"/>
@@ -1609,11 +1891,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1722,7 +1999,7 @@
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
     </row>
-    <row r="11" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
         <v>61</v>
       </c>
@@ -1922,7 +2199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tested the failed test cases
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint 1.xlsx
+++ b/Test-cases/Sprint 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="720" windowWidth="19440" windowHeight="12180" tabRatio="502" activeTab="2"/>
+    <workbookView xWindow="645" yWindow="720" windowWidth="19440" windowHeight="12180" tabRatio="502" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="95">
   <si>
     <t>Username</t>
   </si>
@@ -230,9 +230,6 @@
   </si>
   <si>
     <t>OK</t>
-  </si>
-  <si>
-    <t>NOT OK</t>
   </si>
   <si>
     <t>Test Results</t>
@@ -379,7 +376,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,12 +387,6 @@
       <patternFill patternType="solid">
         <fgColor indexed="31"/>
         <bgColor indexed="44"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -430,7 +421,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -485,15 +476,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -514,6 +496,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1010,11 +998,11 @@
       <c r="B3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
@@ -1023,11 +1011,11 @@
       <c r="B4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
@@ -1040,26 +1028,26 @@
       <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="29"/>
     </row>
     <row r="9" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
@@ -1070,40 +1058,40 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="28" t="s">
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="21" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -1346,11 +1334,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="C3:E3"/>
@@ -1358,6 +1341,11 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter alignWithMargins="0">
@@ -1381,110 +1369,114 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="23">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="26">
-        <v>1</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="24" t="s">
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="23">
+        <v>2</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="24"/>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="26">
-        <v>2</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="23">
+        <v>3</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="24"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="26">
+      <c r="D7" s="29"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="23">
+        <v>4</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="C10" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="26">
-        <v>4</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="29"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="25">
+      <c r="A13" s="22">
         <v>5</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="20" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1509,125 +1501,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="27">
+        <v>1</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="30">
-        <v>1</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="28" t="s">
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="27">
+        <v>2</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="28"/>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="30">
-        <v>2</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="28" t="s">
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="28"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="22" t="s">
+      <c r="D5" s="29"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="27">
+        <v>3</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="30">
+      <c r="D7" s="29"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="29"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="27">
+        <v>4</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="22" t="s">
+      <c r="C10" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="22"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="30">
-        <v>4</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="29"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="29">
+      <c r="A13" s="26">
         <v>5</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="20" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1653,7 +1645,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1685,10 +1677,10 @@
       <c r="B3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
@@ -1697,10 +1689,10 @@
       <c r="B4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="29"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
@@ -1713,34 +1705,34 @@
       <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="29"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
@@ -1751,36 +1743,36 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="28" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="21" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
     </row>
     <row r="14" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
@@ -1799,10 +1791,10 @@
         <v>67</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1821,11 +1813,11 @@
       <c r="E15" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>69</v>
+      <c r="F15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
@@ -1844,11 +1836,11 @@
       <c r="E16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>69</v>
+      <c r="F16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1865,11 +1857,11 @@
       <c r="E17" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>69</v>
+      <c r="F17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1879,11 +1871,6 @@
     <row r="22" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C3:D3"/>
@@ -1891,6 +1878,11 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1938,11 +1930,11 @@
       <c r="B3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
@@ -1951,11 +1943,11 @@
       <c r="B4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
@@ -1968,18 +1960,18 @@
       <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
@@ -1990,10 +1982,10 @@
       <c r="B9" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
@@ -2004,18 +1996,18 @@
         <v>61</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2066,7 +2058,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="14"/>
     </row>
@@ -2081,12 +2073,12 @@
       <c r="B3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="C3" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
@@ -2095,20 +2087,20 @@
       <c r="B4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="22"/>
+      <c r="C5" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
@@ -2119,20 +2111,20 @@
         <v>3</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="22"/>
+      <c r="C8" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="29"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
@@ -2145,14 +2137,14 @@
       <c r="B10" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="22"/>
+      <c r="C10" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="29"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
@@ -2162,18 +2154,18 @@
         <v>61</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C14" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2187,6 +2179,7 @@
     <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2199,8 +2192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2232,11 +2225,11 @@
       <c r="B3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
@@ -2245,11 +2238,11 @@
       <c r="B4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
@@ -2262,18 +2255,18 @@
       <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
@@ -2284,10 +2277,10 @@
       <c r="B9" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
@@ -2298,7 +2291,7 @@
         <v>61</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>68</v>
@@ -2306,7 +2299,7 @@
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>68</v>

</xml_diff>